<commit_message>
DESPUES DE SUBIR ARCHIVOS
</commit_message>
<xml_diff>
--- a/OperadoraNominas/bin/Debug/Archivos/nominas1.xlsx
+++ b/OperadoraNominas/bin/Debug/Archivos/nominas1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7035"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7035" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Generales" sheetId="2" r:id="rId1"/>
@@ -244,7 +244,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="65">
   <si>
     <t>No. Empleado</t>
   </si>
@@ -436,6 +436,9 @@
   </si>
   <si>
     <t>Subsidio Causado</t>
+  </si>
+  <si>
+    <t>NOMBRE</t>
   </si>
 </sst>
 </file>
@@ -794,7 +797,7 @@
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -869,6 +872,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Millares 2" xfId="3"/>
@@ -1277,7 +1281,7 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:AE814"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="I11" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -4140,11 +4144,11 @@
   <sheetPr codeName="Hoja4"/>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4:XFD16"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4172,7 +4176,9 @@
       <c r="A3" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="19"/>
+      <c r="B3" s="40" t="s">
+        <v>64</v>
+      </c>
       <c r="C3" s="20" t="s">
         <v>58</v>
       </c>

</xml_diff>